<commit_message>
add: lógica do template
</commit_message>
<xml_diff>
--- a/Mensageria/betti/email.xlsx
+++ b/Mensageria/betti/email.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.alves\source\aulas\AulasEuCodo\Mensageria\bin\Debug\net6.0\betti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.alves\source\aulas\AulasEuCodo\Mensageria\betti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8575313C-6F36-4F69-AC73-63773187C91E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DD8D5A-16FC-4AEF-83D4-F0862B7F5261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B2C2596-FEDC-4806-AA04-C3A6BED56956}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="43">
   <si>
     <t>A</t>
   </si>
@@ -128,9 +128,6 @@
     <t>William</t>
   </si>
   <si>
-    <t>bulpert@yahoo.com</t>
-  </si>
-  <si>
     <t>jurupis</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>CLIENTE</t>
   </si>
   <si>
-    <t>DESTINATÁRIO</t>
-  </si>
-  <si>
     <t>nayrpkt@gmail.com</t>
   </si>
   <si>
@@ -168,6 +162,9 @@
   </si>
   <si>
     <t>nayrpkt@gmail.com, robert_hk_@hotmail.com</t>
+  </si>
+  <si>
+    <t>EMAIL DO PROJETO</t>
   </si>
 </sst>
 </file>
@@ -540,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59491F56-CD08-47F1-9229-800FA97E9013}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,33 +550,33 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
       <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
         <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -597,15 +594,15 @@
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -623,15 +620,15 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -646,18 +643,18 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -675,15 +672,15 @@
         <v>11</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -701,15 +698,15 @@
         <v>14</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -727,15 +724,15 @@
         <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -753,15 +750,15 @@
         <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -779,15 +776,15 @@
         <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -805,21 +802,21 @@
         <v>26</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="C11">
-        <v>1010</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
@@ -831,21 +828,308 @@
         <v>29</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>101</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>101</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>101</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>101</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19">
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>101</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23">
+        <v>101</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{211C1AE1-1DBC-4DBB-A156-E4CE9FFC88C7}"/>
-    <hyperlink ref="G3:G11" r:id="rId2" display="bulpert@yahoo.com" xr:uid="{CA459344-A753-4D58-A101-40AA3762FF23}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{C64B1445-845E-4D20-8B1F-7CEAE7BCDB55}"/>
-    <hyperlink ref="H2" r:id="rId4" display="nayrpkt@gmail.com" xr:uid="{FCA25B0F-6286-4320-9B1F-FD5A64DBBEB1}"/>
-    <hyperlink ref="H3:H11" r:id="rId5" display="nayrpkt@gmail.com" xr:uid="{1C12571D-C915-4127-BE48-164C42B2BADC}"/>
+    <hyperlink ref="H3:H11" r:id="rId2" display="nayrpkt@gmail.com" xr:uid="{1C12571D-C915-4127-BE48-164C42B2BADC}"/>
+    <hyperlink ref="H2" r:id="rId3" display="nayrpkt@gmail.com" xr:uid="{FCA25B0F-6286-4320-9B1F-FD5A64DBBEB1}"/>
+    <hyperlink ref="G3:G11" r:id="rId4" display="robert.ads.anjos@gmail.com" xr:uid="{00541651-9D2B-43BD-B943-758F742CF890}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{8846D3E7-7F6A-433B-8850-9FE6F710A435}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{D8B72EC1-EAA9-488E-AF90-8B094ACF4DAE}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{9C017440-1F6A-4B72-8AA6-CED944057224}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{BE67361D-E62B-4826-AEC7-E19537DAAAAD}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{694F377E-4292-4105-A106-0ED19C02DA75}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{BAE5F8E1-BBCC-4CA6-806C-851799B38594}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{AEB30C71-9B96-4F83-90F5-49FCBFA5AB31}"/>
+    <hyperlink ref="G19" r:id="rId12" xr:uid="{1DFB4A55-F1D0-48F7-804E-8380FFC89D1D}"/>
+    <hyperlink ref="G20" r:id="rId13" xr:uid="{853FE99F-AFDC-4568-8AE5-6DDDF9F39777}"/>
+    <hyperlink ref="G21" r:id="rId14" xr:uid="{CB9DF868-D144-46D2-A04B-666547E3F045}"/>
+    <hyperlink ref="G22" r:id="rId15" xr:uid="{BC7344BB-1DAD-4366-A981-7EBAD6F632C8}"/>
+    <hyperlink ref="G23" r:id="rId16" xr:uid="{E503B1FB-906B-4E20-92F0-17175E37ADE9}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
condição de unidade x pasta (file)
</commit_message>
<xml_diff>
--- a/Mensageria/betti/email.xlsx
+++ b/Mensageria/betti/email.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.alves\source\aulas\AulasEuCodo\Mensageria\betti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DD8D5A-16FC-4AEF-83D4-F0862B7F5261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956DBF88-F2FE-403A-8651-264447D286A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B2C2596-FEDC-4806-AA04-C3A6BED56956}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
   <si>
     <t>A</t>
   </si>
@@ -537,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59491F56-CD08-47F1-9229-800FA97E9013}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -608,7 +608,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>205</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -634,7 +634,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>307</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -660,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>412</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -686,7 +686,7 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>510</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -712,7 +712,7 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>623</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -738,7 +738,7 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>705</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -764,7 +764,7 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>812</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -790,7 +790,7 @@
         <v>24</v>
       </c>
       <c r="C10">
-        <v>923</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
         <v>25</v>
@@ -816,7 +816,7 @@
         <v>27</v>
       </c>
       <c r="C11">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
@@ -842,7 +842,7 @@
         <v>27</v>
       </c>
       <c r="C12">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
@@ -856,6 +856,9 @@
       <c r="G12" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="H12" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -865,7 +868,7 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -879,6 +882,9 @@
       <c r="G13" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="H13" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -888,7 +894,7 @@
         <v>27</v>
       </c>
       <c r="C14">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
@@ -902,6 +908,9 @@
       <c r="G14" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="H14" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -911,7 +920,7 @@
         <v>27</v>
       </c>
       <c r="C15">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
         <v>28</v>
@@ -925,6 +934,9 @@
       <c r="G15" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="H15" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -934,7 +946,7 @@
         <v>27</v>
       </c>
       <c r="C16">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
         <v>28</v>
@@ -948,8 +960,11 @@
       <c r="G16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -957,7 +972,7 @@
         <v>27</v>
       </c>
       <c r="C17">
-        <v>101</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>28</v>
@@ -971,8 +986,11 @@
       <c r="G17" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -980,7 +998,7 @@
         <v>27</v>
       </c>
       <c r="C18">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>28</v>
@@ -994,8 +1012,11 @@
       <c r="G18" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1003,7 +1024,7 @@
         <v>27</v>
       </c>
       <c r="C19">
-        <v>101</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
@@ -1017,8 +1038,11 @@
       <c r="G19" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1026,7 +1050,7 @@
         <v>27</v>
       </c>
       <c r="C20">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>28</v>
@@ -1040,8 +1064,11 @@
       <c r="G20" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1049,7 +1076,7 @@
         <v>27</v>
       </c>
       <c r="C21">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
@@ -1063,51 +1090,8 @@
       <c r="G21" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22">
-        <v>101</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <v>101</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>31</v>
+      <c r="H21" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1116,20 +1100,28 @@
     <hyperlink ref="H3:H11" r:id="rId2" display="nayrpkt@gmail.com" xr:uid="{1C12571D-C915-4127-BE48-164C42B2BADC}"/>
     <hyperlink ref="H2" r:id="rId3" display="nayrpkt@gmail.com" xr:uid="{FCA25B0F-6286-4320-9B1F-FD5A64DBBEB1}"/>
     <hyperlink ref="G3:G11" r:id="rId4" display="robert.ads.anjos@gmail.com" xr:uid="{00541651-9D2B-43BD-B943-758F742CF890}"/>
-    <hyperlink ref="G12" r:id="rId5" xr:uid="{8846D3E7-7F6A-433B-8850-9FE6F710A435}"/>
-    <hyperlink ref="G13" r:id="rId6" xr:uid="{D8B72EC1-EAA9-488E-AF90-8B094ACF4DAE}"/>
-    <hyperlink ref="G14" r:id="rId7" xr:uid="{9C017440-1F6A-4B72-8AA6-CED944057224}"/>
-    <hyperlink ref="G15" r:id="rId8" xr:uid="{BE67361D-E62B-4826-AEC7-E19537DAAAAD}"/>
-    <hyperlink ref="G16" r:id="rId9" xr:uid="{694F377E-4292-4105-A106-0ED19C02DA75}"/>
-    <hyperlink ref="G17" r:id="rId10" xr:uid="{BAE5F8E1-BBCC-4CA6-806C-851799B38594}"/>
-    <hyperlink ref="G18" r:id="rId11" xr:uid="{AEB30C71-9B96-4F83-90F5-49FCBFA5AB31}"/>
-    <hyperlink ref="G19" r:id="rId12" xr:uid="{1DFB4A55-F1D0-48F7-804E-8380FFC89D1D}"/>
-    <hyperlink ref="G20" r:id="rId13" xr:uid="{853FE99F-AFDC-4568-8AE5-6DDDF9F39777}"/>
-    <hyperlink ref="G21" r:id="rId14" xr:uid="{CB9DF868-D144-46D2-A04B-666547E3F045}"/>
-    <hyperlink ref="G22" r:id="rId15" xr:uid="{BC7344BB-1DAD-4366-A981-7EBAD6F632C8}"/>
-    <hyperlink ref="G23" r:id="rId16" xr:uid="{E503B1FB-906B-4E20-92F0-17175E37ADE9}"/>
+    <hyperlink ref="H12" r:id="rId5" xr:uid="{D58CF81B-0951-42A7-B4CC-E4A6F9A89509}"/>
+    <hyperlink ref="H13" r:id="rId6" xr:uid="{7F260C45-0D77-442C-B97D-6F74E84A36D7}"/>
+    <hyperlink ref="H14" r:id="rId7" xr:uid="{09AE1589-F8A7-4F1B-8816-D0C5B35F40E5}"/>
+    <hyperlink ref="H15" r:id="rId8" xr:uid="{AA8EFC28-19EC-408D-B1EE-53E23075A590}"/>
+    <hyperlink ref="H16" r:id="rId9" xr:uid="{917A5642-E1A6-4314-8F64-09963EE0C884}"/>
+    <hyperlink ref="H17" r:id="rId10" xr:uid="{3E781638-FB69-4324-9B8D-1C4F01A3A221}"/>
+    <hyperlink ref="H18" r:id="rId11" xr:uid="{BA93F156-3629-4F73-ABD2-778848B088FD}"/>
+    <hyperlink ref="H19" r:id="rId12" xr:uid="{A22BD2D9-9706-42F2-B0ED-5D70FA342FD2}"/>
+    <hyperlink ref="H20" r:id="rId13" xr:uid="{CCC9C050-6E08-49A3-909E-EB73177D03C0}"/>
+    <hyperlink ref="H21" r:id="rId14" xr:uid="{5291E255-C510-4237-9CCD-E0DBCCABC219}"/>
+    <hyperlink ref="G12" r:id="rId15" xr:uid="{F5D11A7A-D37E-4408-B5AC-27B3EF698B20}"/>
+    <hyperlink ref="G13" r:id="rId16" xr:uid="{DD1E2D4C-327C-4990-961B-BC5A7018D85D}"/>
+    <hyperlink ref="G14" r:id="rId17" xr:uid="{1939887B-716D-45CD-A82D-4F04EF8386FD}"/>
+    <hyperlink ref="G15" r:id="rId18" xr:uid="{D23DD955-1E4C-470B-A94A-3967ECB3D632}"/>
+    <hyperlink ref="G16" r:id="rId19" xr:uid="{E5D6502F-51E8-4EC8-925A-9CEC53E3E6A0}"/>
+    <hyperlink ref="G17" r:id="rId20" xr:uid="{FFC28591-5153-4225-AAD3-E85CBD0CD567}"/>
+    <hyperlink ref="G18" r:id="rId21" xr:uid="{CF10A5C2-A509-469A-817A-7DF1409C9FFD}"/>
+    <hyperlink ref="G19" r:id="rId22" xr:uid="{F69C18C0-F992-4478-B99F-A115AD37C4FC}"/>
+    <hyperlink ref="G20" r:id="rId23" xr:uid="{D784AD20-00A5-4F76-AEBD-01594C6FCDFF}"/>
+    <hyperlink ref="G21" r:id="rId24" xr:uid="{F9956A11-15E4-47F8-894C-D00F02DC0AD0}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alterando o parâmetro destino.
</commit_message>
<xml_diff>
--- a/Mensageria/betti/email.xlsx
+++ b/Mensageria/betti/email.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.alves\source\aulas\AulasEuCodo\Mensageria\betti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B2E975-0251-4B33-B51D-C72761D34AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AAE4BE-CC0F-4CF5-AAFC-7A7CEC277558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B2C2596-FEDC-4806-AA04-C3A6BED56956}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="40">
   <si>
     <t>A</t>
   </si>
@@ -519,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59491F56-CD08-47F1-9229-800FA97E9013}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,14 +790,1666 @@
         <v>36</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>34</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>36</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44">
+        <v>43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46">
+        <v>45</v>
+      </c>
+      <c r="D46" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47">
+        <v>46</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49">
+        <v>48</v>
+      </c>
+      <c r="D49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50">
+        <v>49</v>
+      </c>
+      <c r="D50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51">
+        <v>50</v>
+      </c>
+      <c r="D51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C52">
+        <v>51</v>
+      </c>
+      <c r="D52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53">
+        <v>52</v>
+      </c>
+      <c r="D53" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54">
+        <v>53</v>
+      </c>
+      <c r="D54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" t="s">
+        <v>26</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55">
+        <v>54</v>
+      </c>
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56">
+        <v>55</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" t="s">
+        <v>26</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E57" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" t="s">
+        <v>26</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58">
+        <v>57</v>
+      </c>
+      <c r="D58" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59">
+        <v>58</v>
+      </c>
+      <c r="D59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C60">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61">
+        <v>60</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" t="s">
+        <v>26</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62">
+        <v>61</v>
+      </c>
+      <c r="D62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63">
+        <v>62</v>
+      </c>
+      <c r="D63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64">
+        <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>25</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
+        <v>26</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66">
+        <v>65</v>
+      </c>
+      <c r="D66" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67">
+        <v>66</v>
+      </c>
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" t="s">
+        <v>26</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68">
+        <v>67</v>
+      </c>
+      <c r="D68" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" t="s">
+        <v>26</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69">
+        <v>68</v>
+      </c>
+      <c r="D69" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" t="s">
+        <v>26</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{211C1AE1-1DBC-4DBB-A156-E4CE9FFC88C7}"/>
     <hyperlink ref="H3:H10" r:id="rId2" display="nayrpkt@gmail.com" xr:uid="{1C12571D-C915-4127-BE48-164C42B2BADC}"/>
     <hyperlink ref="H2" r:id="rId3" display="nayrpkt@gmail.com" xr:uid="{FCA25B0F-6286-4320-9B1F-FD5A64DBBEB1}"/>
     <hyperlink ref="G3:G10" r:id="rId4" display="robert.ads.anjos@gmail.com" xr:uid="{00541651-9D2B-43BD-B943-758F742CF890}"/>
+    <hyperlink ref="H11" r:id="rId5" xr:uid="{09910E8B-CFB6-4993-BE95-18D6BF11E190}"/>
+    <hyperlink ref="H12" r:id="rId6" xr:uid="{8610FAB9-5999-4A38-871D-4C1AE88D7923}"/>
+    <hyperlink ref="H13" r:id="rId7" xr:uid="{C946FAFE-0CF1-43DB-9803-E3ABF5958E7A}"/>
+    <hyperlink ref="H14" r:id="rId8" xr:uid="{28B25D6C-D4C2-4BD9-9186-F9A8748940AD}"/>
+    <hyperlink ref="H15" r:id="rId9" xr:uid="{3B765E08-3291-4178-B3E9-D2C079CC4B5A}"/>
+    <hyperlink ref="H16" r:id="rId10" xr:uid="{04969B02-7E9A-4733-AF4C-F29780CED7DA}"/>
+    <hyperlink ref="H17" r:id="rId11" xr:uid="{B59896AB-E253-4497-8693-6C5CD2B25FAF}"/>
+    <hyperlink ref="H18" r:id="rId12" xr:uid="{E25808FE-B1C8-471E-9A2F-0FC8B65D12BC}"/>
+    <hyperlink ref="H19" r:id="rId13" xr:uid="{90096C27-04B4-4EF5-96C7-37D31B7AA5F9}"/>
+    <hyperlink ref="H20" r:id="rId14" xr:uid="{1408B4ED-C8DB-4E2E-B95F-8E2802D47C7A}"/>
+    <hyperlink ref="H21" r:id="rId15" xr:uid="{83788C3C-2E79-41D9-B076-09053A1FC036}"/>
+    <hyperlink ref="H22" r:id="rId16" xr:uid="{EB81B099-701F-4F79-AB9E-23C3299060AB}"/>
+    <hyperlink ref="H23" r:id="rId17" xr:uid="{6D15EDAF-833F-42FE-928B-C27ED961EC77}"/>
+    <hyperlink ref="H24" r:id="rId18" xr:uid="{5727F37F-098A-4636-B56E-C754B8BBEF8C}"/>
+    <hyperlink ref="H25" r:id="rId19" xr:uid="{FB8C61C4-1DDB-4228-A817-C4DA780BEB44}"/>
+    <hyperlink ref="H26" r:id="rId20" xr:uid="{DB2501ED-C61B-40F0-A3A2-2A80B107804E}"/>
+    <hyperlink ref="H27" r:id="rId21" xr:uid="{E2E87CB7-C7A4-42D8-AED1-4DE641E0D342}"/>
+    <hyperlink ref="H28" r:id="rId22" xr:uid="{5406506C-B336-4BDC-A0AF-1FB8BD0EA880}"/>
+    <hyperlink ref="H29" r:id="rId23" xr:uid="{BB77BA83-9818-43A6-A600-A5642D848870}"/>
+    <hyperlink ref="H30" r:id="rId24" xr:uid="{E68A039C-A287-4F27-BB9D-B84C3A44D3CF}"/>
+    <hyperlink ref="H31" r:id="rId25" xr:uid="{462964A2-5D01-4B51-9EDD-96DA2989A4A7}"/>
+    <hyperlink ref="H32" r:id="rId26" xr:uid="{515F2F48-0AC8-45BA-A768-A546FED53777}"/>
+    <hyperlink ref="H33" r:id="rId27" xr:uid="{1361260E-44D7-4F0B-A49F-98E32870F847}"/>
+    <hyperlink ref="H34" r:id="rId28" xr:uid="{60C852E4-6A62-43DD-9F6F-B04F128919BB}"/>
+    <hyperlink ref="H35" r:id="rId29" xr:uid="{E8A002E2-B988-4D76-8829-E7064240C772}"/>
+    <hyperlink ref="H36" r:id="rId30" xr:uid="{54B7A8C9-1E1B-4E3F-8AEA-E2B80465FF5B}"/>
+    <hyperlink ref="H37" r:id="rId31" xr:uid="{6605C19A-361D-4F7F-923C-B0B2CD9461C5}"/>
+    <hyperlink ref="H38" r:id="rId32" xr:uid="{CD9455D7-E6FE-44C4-87DD-A145099CA99C}"/>
+    <hyperlink ref="H39" r:id="rId33" xr:uid="{6D4F794E-6D23-4ABF-8AA4-EA1BCD777FB7}"/>
+    <hyperlink ref="H40" r:id="rId34" xr:uid="{6901E312-FF6A-437C-8E23-A3C3A7A6D06F}"/>
+    <hyperlink ref="H41" r:id="rId35" xr:uid="{C110BBBB-B163-4E4A-BA61-EF21F97C048A}"/>
+    <hyperlink ref="H42" r:id="rId36" xr:uid="{ADCD7D38-7927-47F0-80B3-66B9E8D935D6}"/>
+    <hyperlink ref="H43" r:id="rId37" xr:uid="{954E0104-7867-4219-A2D9-1906FAF6FEF1}"/>
+    <hyperlink ref="H44" r:id="rId38" xr:uid="{69945E1F-0483-4ABF-93A0-CAB64F0DC480}"/>
+    <hyperlink ref="H45" r:id="rId39" xr:uid="{B7E5EE66-6A24-48B3-95DA-541131D194E5}"/>
+    <hyperlink ref="H46" r:id="rId40" xr:uid="{F42004BC-3292-40C4-B85F-78A5FFC0575E}"/>
+    <hyperlink ref="H47" r:id="rId41" xr:uid="{2DA0B9FA-F04D-47CD-AC45-1648382DE809}"/>
+    <hyperlink ref="H48" r:id="rId42" xr:uid="{ED3BFEE6-4FB3-44C0-825A-04E54EFBC4DD}"/>
+    <hyperlink ref="H49" r:id="rId43" xr:uid="{2B265C5B-C51B-4FA1-956E-5A340EE815AD}"/>
+    <hyperlink ref="H50" r:id="rId44" xr:uid="{1D966E29-2556-4CC1-9525-BCB7D76B5B83}"/>
+    <hyperlink ref="H51" r:id="rId45" xr:uid="{D2E9BAA9-EF2E-4D5C-8B0C-A8E18C472C3A}"/>
+    <hyperlink ref="H52" r:id="rId46" xr:uid="{371B6130-EBEE-4A37-9A6D-91E7E6D1F2FD}"/>
+    <hyperlink ref="H53" r:id="rId47" xr:uid="{D2261BFB-94B8-438F-B14E-71DB9A3961D0}"/>
+    <hyperlink ref="H54" r:id="rId48" xr:uid="{E603B97B-61EC-4F16-9999-DE40CD3FF60F}"/>
+    <hyperlink ref="H55" r:id="rId49" xr:uid="{C7840E43-F2D8-49CB-B717-B065C321006E}"/>
+    <hyperlink ref="H56" r:id="rId50" xr:uid="{EA51FE1A-034F-4738-9B13-DD7FC2BEA0AE}"/>
+    <hyperlink ref="H57" r:id="rId51" xr:uid="{EA0D4843-A2A2-4EE9-BD56-5BF0CF26C6ED}"/>
+    <hyperlink ref="H58" r:id="rId52" xr:uid="{5F15A054-9654-43DE-A310-A281363B867E}"/>
+    <hyperlink ref="H59" r:id="rId53" xr:uid="{2AAD2FC9-7875-4C7E-BE18-5929DCD300E2}"/>
+    <hyperlink ref="H60" r:id="rId54" xr:uid="{3B13B48B-CFD8-43FD-A256-BFBCA6E9F166}"/>
+    <hyperlink ref="H61" r:id="rId55" xr:uid="{2812F3C5-BA5B-4280-A6EE-F071C743A0F9}"/>
+    <hyperlink ref="H62" r:id="rId56" xr:uid="{A51391BB-726E-4E53-A854-F835E4326CB7}"/>
+    <hyperlink ref="H63" r:id="rId57" xr:uid="{3816078E-236A-40ED-8098-8D6C2593073C}"/>
+    <hyperlink ref="H64" r:id="rId58" xr:uid="{16019511-2A5B-45DB-9951-7580C7CED611}"/>
+    <hyperlink ref="H65" r:id="rId59" xr:uid="{0F281052-88CC-4EFC-9654-D738A5265195}"/>
+    <hyperlink ref="H66" r:id="rId60" xr:uid="{988320DB-75EE-40A5-80AB-5DC5D88C77B3}"/>
+    <hyperlink ref="H67" r:id="rId61" xr:uid="{BD69E281-B932-4E39-BC3D-0A5839B363E1}"/>
+    <hyperlink ref="H68" r:id="rId62" xr:uid="{E063F8A8-C725-4BE8-8357-391DBDD95480}"/>
+    <hyperlink ref="H69" r:id="rId63" xr:uid="{46926277-A148-4D82-AF7C-43360CBCA36A}"/>
+    <hyperlink ref="G11" r:id="rId64" xr:uid="{08891F1E-BFCE-4901-BB79-93AA85608BD6}"/>
+    <hyperlink ref="G12" r:id="rId65" xr:uid="{5B945965-8CF2-4536-B6C6-B03AA77AC55C}"/>
+    <hyperlink ref="G13" r:id="rId66" xr:uid="{474F2900-37DB-45FC-AC64-A44473756317}"/>
+    <hyperlink ref="G14" r:id="rId67" xr:uid="{8083D30B-557A-4AC8-8D3C-27A3DD20F6F0}"/>
+    <hyperlink ref="G15" r:id="rId68" xr:uid="{9BC24074-15A2-42CF-82F3-9EE884921304}"/>
+    <hyperlink ref="G16" r:id="rId69" xr:uid="{CC4BD510-687D-4365-A02B-40308B7BB094}"/>
+    <hyperlink ref="G17" r:id="rId70" xr:uid="{307F9D09-DD1B-449E-8BD1-CEA8554CE58F}"/>
+    <hyperlink ref="G18" r:id="rId71" xr:uid="{256E56A0-313B-40C0-B777-463B070E8BC5}"/>
+    <hyperlink ref="G19" r:id="rId72" xr:uid="{53093AA6-4084-4A8D-9497-0ED7AA03C383}"/>
+    <hyperlink ref="G20" r:id="rId73" xr:uid="{0A61BB15-6DA2-4651-832C-63B5FBFBF363}"/>
+    <hyperlink ref="G21" r:id="rId74" xr:uid="{81605D05-A6AE-48A8-B253-5F4DDBDA4ADF}"/>
+    <hyperlink ref="G22" r:id="rId75" xr:uid="{CC010305-21EE-4FDA-9CD9-E1E88E21073E}"/>
+    <hyperlink ref="G23" r:id="rId76" xr:uid="{015C4D36-070E-4AE5-8A75-18BB99358F8A}"/>
+    <hyperlink ref="G24" r:id="rId77" xr:uid="{9388E673-BA81-47E0-BFEB-FD5D9EFB6189}"/>
+    <hyperlink ref="G25" r:id="rId78" xr:uid="{C35AD358-FAE5-4651-BA71-7FCB62B777AD}"/>
+    <hyperlink ref="G26" r:id="rId79" xr:uid="{49164CC9-A989-48A1-907E-506CF71CAD23}"/>
+    <hyperlink ref="G27" r:id="rId80" xr:uid="{FD0CC0A5-6781-4196-BC44-A37E10AEC42E}"/>
+    <hyperlink ref="G28" r:id="rId81" xr:uid="{EEC82DBC-4EC1-4487-B9D7-395DEF439593}"/>
+    <hyperlink ref="G29" r:id="rId82" xr:uid="{D76B3FB4-0C70-4CE6-918B-0908E0F374B8}"/>
+    <hyperlink ref="G30" r:id="rId83" xr:uid="{1DEFF231-CA99-4D17-8AE5-615AC7A823A4}"/>
+    <hyperlink ref="G31" r:id="rId84" xr:uid="{966D5DAB-BC05-48B1-AED4-A984DDFA9687}"/>
+    <hyperlink ref="G32" r:id="rId85" xr:uid="{89CC95B8-463D-4ED6-BCD0-BD61431EEC6B}"/>
+    <hyperlink ref="G33" r:id="rId86" xr:uid="{59E52C85-2003-40A5-8C17-8E2F50167809}"/>
+    <hyperlink ref="G34" r:id="rId87" xr:uid="{BA71EEF9-AF74-4964-81CA-5687E31C1DD4}"/>
+    <hyperlink ref="G35" r:id="rId88" xr:uid="{D4B8B830-7DBB-47C0-A575-21C20C37106F}"/>
+    <hyperlink ref="G36" r:id="rId89" xr:uid="{A3B66E16-DF2D-4C8E-8493-576C3B334E63}"/>
+    <hyperlink ref="G37" r:id="rId90" xr:uid="{A8760C98-A87A-41BC-846D-7C27B64DC83F}"/>
+    <hyperlink ref="G38" r:id="rId91" xr:uid="{A325DB0A-16B9-4C9B-AD23-028436D268E4}"/>
+    <hyperlink ref="G39" r:id="rId92" xr:uid="{21E4E18D-D7B0-4619-9131-F214640DD643}"/>
+    <hyperlink ref="G40" r:id="rId93" xr:uid="{BB72CDF5-7DBF-4D40-BD56-FA7B73CD3590}"/>
+    <hyperlink ref="G41" r:id="rId94" xr:uid="{0755F9B0-B3FA-4412-9627-511B01D587C4}"/>
+    <hyperlink ref="G42" r:id="rId95" xr:uid="{0E77696F-C2A8-46A4-A1C9-5B053BCCD56A}"/>
+    <hyperlink ref="G43" r:id="rId96" xr:uid="{62AD8424-5EED-4E05-BD4A-67FFF079F5DE}"/>
+    <hyperlink ref="G44" r:id="rId97" xr:uid="{BD5F52DA-750A-4708-9209-F0832953610C}"/>
+    <hyperlink ref="G45" r:id="rId98" xr:uid="{5DB21C96-F541-4875-82E0-FD95E99F7A16}"/>
+    <hyperlink ref="G46" r:id="rId99" xr:uid="{3296534A-C4DB-4629-8892-2512BE67C1E1}"/>
+    <hyperlink ref="G47" r:id="rId100" xr:uid="{FC4C2567-5D0A-4A46-87FD-0F052C0C538D}"/>
+    <hyperlink ref="G48" r:id="rId101" xr:uid="{CCBD4575-042B-483B-B95F-DB0C6BFBBF8D}"/>
+    <hyperlink ref="G49" r:id="rId102" xr:uid="{433D9299-B965-440B-AB9D-D1BC0FF90227}"/>
+    <hyperlink ref="G50" r:id="rId103" xr:uid="{9C92CA39-C795-4745-BCA7-75F9635352EF}"/>
+    <hyperlink ref="G51" r:id="rId104" xr:uid="{80955053-99B6-4770-9451-1AB0C4AB0658}"/>
+    <hyperlink ref="G52" r:id="rId105" xr:uid="{D08F8A10-1FEA-4FF8-91AA-4D5C6E2CF965}"/>
+    <hyperlink ref="G53" r:id="rId106" xr:uid="{E1552DE5-3F36-4447-A098-1C38DEF076C3}"/>
+    <hyperlink ref="G54" r:id="rId107" xr:uid="{27C89CBD-A689-49D7-A356-45AB8D080E30}"/>
+    <hyperlink ref="G55" r:id="rId108" xr:uid="{71744331-B135-4284-A969-858AB98596A0}"/>
+    <hyperlink ref="G56" r:id="rId109" xr:uid="{E8227959-A688-47B5-8A00-EAAE316BCF25}"/>
+    <hyperlink ref="G57" r:id="rId110" xr:uid="{81A75D53-81AF-47EF-955C-7F6AE6E8D441}"/>
+    <hyperlink ref="G58" r:id="rId111" xr:uid="{381AF0E9-4678-4C36-98E5-18D44A2CC57D}"/>
+    <hyperlink ref="G59" r:id="rId112" xr:uid="{851C0207-0075-4165-8E96-8EDBA705D1BE}"/>
+    <hyperlink ref="G60" r:id="rId113" xr:uid="{0EB71C1A-846F-471B-A44E-D6A98021B2BD}"/>
+    <hyperlink ref="G61" r:id="rId114" xr:uid="{015E38E2-E0E0-4C07-9DC8-737D165A1996}"/>
+    <hyperlink ref="G62" r:id="rId115" xr:uid="{403E4063-551A-486E-A1F9-3F42AF284878}"/>
+    <hyperlink ref="G63" r:id="rId116" xr:uid="{4B58B3D6-A744-4480-9F2D-E188A123B412}"/>
+    <hyperlink ref="G64" r:id="rId117" xr:uid="{8042DD29-EA9B-4FD4-82D4-4821278FDA07}"/>
+    <hyperlink ref="G65" r:id="rId118" xr:uid="{C726FBED-BFBE-4CE0-96C2-8969080BF41C}"/>
+    <hyperlink ref="G66" r:id="rId119" xr:uid="{A7FDEECE-9C08-46A0-9503-19049D241A3B}"/>
+    <hyperlink ref="G67" r:id="rId120" xr:uid="{8A8FED6A-5191-4D66-9581-4022B7D0D290}"/>
+    <hyperlink ref="G68" r:id="rId121" xr:uid="{A08C4575-38E9-451E-80D2-24708329B4C0}"/>
+    <hyperlink ref="G69" r:id="rId122" xr:uid="{72CA6DCC-6E4F-454E-BE85-9513BC2C22F5}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId123"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mecanismo para CC implementado com sucesso!
</commit_message>
<xml_diff>
--- a/Mensageria/betti/email.xlsx
+++ b/Mensageria/betti/email.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.alves\source\aulas\AulasEuCodo\Mensageria\betti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AAE4BE-CC0F-4CF5-AAFC-7A7CEC277558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECEB8B-8EB5-47B6-A844-C7DB66593508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B2C2596-FEDC-4806-AA04-C3A6BED56956}"/>
   </bookViews>
@@ -128,9 +128,6 @@
     <t>Jubuscléia</t>
   </si>
   <si>
-    <t>PASTA</t>
-  </si>
-  <si>
     <t>TORRE</t>
   </si>
   <si>
@@ -146,16 +143,19 @@
     <t>CLIENTE</t>
   </si>
   <si>
-    <t>nayrpkt@gmail.com</t>
-  </si>
-  <si>
     <t>EMAILS EM CÓPIA (se tiver mais que um, separar por virgula</t>
   </si>
   <si>
-    <t>nayrpkt@gmail.com, robert_hk_@hotmail.com</t>
-  </si>
-  <si>
     <t>EMAIL DO PROJETO</t>
+  </si>
+  <si>
+    <t>PASTA | EMPREENDIMENTO</t>
+  </si>
+  <si>
+    <t>bulpert@yahoo.com, robert_hk_@hotmail.com</t>
+  </si>
+  <si>
+    <t>bulpert@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -521,39 +521,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59491F56-CD08-47F1-9229-800FA97E9013}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
     <col min="8" max="8" width="58.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -605,7 +606,7 @@
         <v>28</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -631,7 +632,7 @@
         <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -657,7 +658,7 @@
         <v>28</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -683,7 +684,7 @@
         <v>28</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -709,7 +710,7 @@
         <v>28</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -735,7 +736,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -761,7 +762,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -787,7 +788,7 @@
         <v>28</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -813,7 +814,7 @@
         <v>28</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -839,7 +840,7 @@
         <v>28</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -865,7 +866,7 @@
         <v>28</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -891,7 +892,7 @@
         <v>28</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -917,7 +918,7 @@
         <v>28</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -943,7 +944,7 @@
         <v>28</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -969,7 +970,7 @@
         <v>28</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -995,7 +996,7 @@
         <v>28</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1021,7 +1022,7 @@
         <v>28</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1047,7 +1048,7 @@
         <v>28</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1073,7 +1074,7 @@
         <v>28</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1099,7 +1100,7 @@
         <v>28</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1125,7 +1126,7 @@
         <v>28</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1151,7 +1152,7 @@
         <v>28</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1177,7 +1178,7 @@
         <v>28</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1203,7 +1204,7 @@
         <v>28</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1229,7 +1230,7 @@
         <v>28</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1255,7 +1256,7 @@
         <v>28</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1281,7 +1282,7 @@
         <v>28</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -1307,7 +1308,7 @@
         <v>28</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -1333,7 +1334,7 @@
         <v>28</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -1359,7 +1360,7 @@
         <v>28</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -1385,7 +1386,7 @@
         <v>28</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -1411,7 +1412,7 @@
         <v>28</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1437,7 +1438,7 @@
         <v>28</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -1463,7 +1464,7 @@
         <v>28</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -1489,7 +1490,7 @@
         <v>28</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -1515,7 +1516,7 @@
         <v>28</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -1541,7 +1542,7 @@
         <v>28</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -1567,7 +1568,7 @@
         <v>28</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -1593,7 +1594,7 @@
         <v>28</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1619,7 +1620,7 @@
         <v>28</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -1645,7 +1646,7 @@
         <v>28</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -1671,7 +1672,7 @@
         <v>28</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -1697,7 +1698,7 @@
         <v>28</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -1723,7 +1724,7 @@
         <v>28</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -1749,7 +1750,7 @@
         <v>28</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -1775,7 +1776,7 @@
         <v>28</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
@@ -1801,7 +1802,7 @@
         <v>28</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -1827,7 +1828,7 @@
         <v>28</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
@@ -1853,7 +1854,7 @@
         <v>28</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
@@ -1879,7 +1880,7 @@
         <v>28</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -1905,7 +1906,7 @@
         <v>28</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -1931,7 +1932,7 @@
         <v>28</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -1957,7 +1958,7 @@
         <v>28</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -1983,7 +1984,7 @@
         <v>28</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -2009,7 +2010,7 @@
         <v>28</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -2035,7 +2036,7 @@
         <v>28</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
@@ -2061,7 +2062,7 @@
         <v>28</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
@@ -2087,7 +2088,7 @@
         <v>28</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -2113,7 +2114,7 @@
         <v>28</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
@@ -2139,7 +2140,7 @@
         <v>28</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -2165,7 +2166,7 @@
         <v>28</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -2191,7 +2192,7 @@
         <v>28</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -2217,7 +2218,7 @@
         <v>28</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -2243,7 +2244,7 @@
         <v>28</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -2269,7 +2270,7 @@
         <v>28</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -2295,7 +2296,7 @@
         <v>28</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -2321,135 +2322,78 @@
         <v>28</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{211C1AE1-1DBC-4DBB-A156-E4CE9FFC88C7}"/>
-    <hyperlink ref="H3:H10" r:id="rId2" display="nayrpkt@gmail.com" xr:uid="{1C12571D-C915-4127-BE48-164C42B2BADC}"/>
-    <hyperlink ref="H2" r:id="rId3" display="nayrpkt@gmail.com" xr:uid="{FCA25B0F-6286-4320-9B1F-FD5A64DBBEB1}"/>
-    <hyperlink ref="G3:G10" r:id="rId4" display="robert.ads.anjos@gmail.com" xr:uid="{00541651-9D2B-43BD-B943-758F742CF890}"/>
-    <hyperlink ref="H11" r:id="rId5" xr:uid="{09910E8B-CFB6-4993-BE95-18D6BF11E190}"/>
-    <hyperlink ref="H12" r:id="rId6" xr:uid="{8610FAB9-5999-4A38-871D-4C1AE88D7923}"/>
-    <hyperlink ref="H13" r:id="rId7" xr:uid="{C946FAFE-0CF1-43DB-9803-E3ABF5958E7A}"/>
-    <hyperlink ref="H14" r:id="rId8" xr:uid="{28B25D6C-D4C2-4BD9-9186-F9A8748940AD}"/>
-    <hyperlink ref="H15" r:id="rId9" xr:uid="{3B765E08-3291-4178-B3E9-D2C079CC4B5A}"/>
-    <hyperlink ref="H16" r:id="rId10" xr:uid="{04969B02-7E9A-4733-AF4C-F29780CED7DA}"/>
-    <hyperlink ref="H17" r:id="rId11" xr:uid="{B59896AB-E253-4497-8693-6C5CD2B25FAF}"/>
-    <hyperlink ref="H18" r:id="rId12" xr:uid="{E25808FE-B1C8-471E-9A2F-0FC8B65D12BC}"/>
-    <hyperlink ref="H19" r:id="rId13" xr:uid="{90096C27-04B4-4EF5-96C7-37D31B7AA5F9}"/>
-    <hyperlink ref="H20" r:id="rId14" xr:uid="{1408B4ED-C8DB-4E2E-B95F-8E2802D47C7A}"/>
-    <hyperlink ref="H21" r:id="rId15" xr:uid="{83788C3C-2E79-41D9-B076-09053A1FC036}"/>
-    <hyperlink ref="H22" r:id="rId16" xr:uid="{EB81B099-701F-4F79-AB9E-23C3299060AB}"/>
-    <hyperlink ref="H23" r:id="rId17" xr:uid="{6D15EDAF-833F-42FE-928B-C27ED961EC77}"/>
-    <hyperlink ref="H24" r:id="rId18" xr:uid="{5727F37F-098A-4636-B56E-C754B8BBEF8C}"/>
-    <hyperlink ref="H25" r:id="rId19" xr:uid="{FB8C61C4-1DDB-4228-A817-C4DA780BEB44}"/>
-    <hyperlink ref="H26" r:id="rId20" xr:uid="{DB2501ED-C61B-40F0-A3A2-2A80B107804E}"/>
-    <hyperlink ref="H27" r:id="rId21" xr:uid="{E2E87CB7-C7A4-42D8-AED1-4DE641E0D342}"/>
-    <hyperlink ref="H28" r:id="rId22" xr:uid="{5406506C-B336-4BDC-A0AF-1FB8BD0EA880}"/>
-    <hyperlink ref="H29" r:id="rId23" xr:uid="{BB77BA83-9818-43A6-A600-A5642D848870}"/>
-    <hyperlink ref="H30" r:id="rId24" xr:uid="{E68A039C-A287-4F27-BB9D-B84C3A44D3CF}"/>
-    <hyperlink ref="H31" r:id="rId25" xr:uid="{462964A2-5D01-4B51-9EDD-96DA2989A4A7}"/>
-    <hyperlink ref="H32" r:id="rId26" xr:uid="{515F2F48-0AC8-45BA-A768-A546FED53777}"/>
-    <hyperlink ref="H33" r:id="rId27" xr:uid="{1361260E-44D7-4F0B-A49F-98E32870F847}"/>
-    <hyperlink ref="H34" r:id="rId28" xr:uid="{60C852E4-6A62-43DD-9F6F-B04F128919BB}"/>
-    <hyperlink ref="H35" r:id="rId29" xr:uid="{E8A002E2-B988-4D76-8829-E7064240C772}"/>
-    <hyperlink ref="H36" r:id="rId30" xr:uid="{54B7A8C9-1E1B-4E3F-8AEA-E2B80465FF5B}"/>
-    <hyperlink ref="H37" r:id="rId31" xr:uid="{6605C19A-361D-4F7F-923C-B0B2CD9461C5}"/>
-    <hyperlink ref="H38" r:id="rId32" xr:uid="{CD9455D7-E6FE-44C4-87DD-A145099CA99C}"/>
-    <hyperlink ref="H39" r:id="rId33" xr:uid="{6D4F794E-6D23-4ABF-8AA4-EA1BCD777FB7}"/>
-    <hyperlink ref="H40" r:id="rId34" xr:uid="{6901E312-FF6A-437C-8E23-A3C3A7A6D06F}"/>
-    <hyperlink ref="H41" r:id="rId35" xr:uid="{C110BBBB-B163-4E4A-BA61-EF21F97C048A}"/>
-    <hyperlink ref="H42" r:id="rId36" xr:uid="{ADCD7D38-7927-47F0-80B3-66B9E8D935D6}"/>
-    <hyperlink ref="H43" r:id="rId37" xr:uid="{954E0104-7867-4219-A2D9-1906FAF6FEF1}"/>
-    <hyperlink ref="H44" r:id="rId38" xr:uid="{69945E1F-0483-4ABF-93A0-CAB64F0DC480}"/>
-    <hyperlink ref="H45" r:id="rId39" xr:uid="{B7E5EE66-6A24-48B3-95DA-541131D194E5}"/>
-    <hyperlink ref="H46" r:id="rId40" xr:uid="{F42004BC-3292-40C4-B85F-78A5FFC0575E}"/>
-    <hyperlink ref="H47" r:id="rId41" xr:uid="{2DA0B9FA-F04D-47CD-AC45-1648382DE809}"/>
-    <hyperlink ref="H48" r:id="rId42" xr:uid="{ED3BFEE6-4FB3-44C0-825A-04E54EFBC4DD}"/>
-    <hyperlink ref="H49" r:id="rId43" xr:uid="{2B265C5B-C51B-4FA1-956E-5A340EE815AD}"/>
-    <hyperlink ref="H50" r:id="rId44" xr:uid="{1D966E29-2556-4CC1-9525-BCB7D76B5B83}"/>
-    <hyperlink ref="H51" r:id="rId45" xr:uid="{D2E9BAA9-EF2E-4D5C-8B0C-A8E18C472C3A}"/>
-    <hyperlink ref="H52" r:id="rId46" xr:uid="{371B6130-EBEE-4A37-9A6D-91E7E6D1F2FD}"/>
-    <hyperlink ref="H53" r:id="rId47" xr:uid="{D2261BFB-94B8-438F-B14E-71DB9A3961D0}"/>
-    <hyperlink ref="H54" r:id="rId48" xr:uid="{E603B97B-61EC-4F16-9999-DE40CD3FF60F}"/>
-    <hyperlink ref="H55" r:id="rId49" xr:uid="{C7840E43-F2D8-49CB-B717-B065C321006E}"/>
-    <hyperlink ref="H56" r:id="rId50" xr:uid="{EA51FE1A-034F-4738-9B13-DD7FC2BEA0AE}"/>
-    <hyperlink ref="H57" r:id="rId51" xr:uid="{EA0D4843-A2A2-4EE9-BD56-5BF0CF26C6ED}"/>
-    <hyperlink ref="H58" r:id="rId52" xr:uid="{5F15A054-9654-43DE-A310-A281363B867E}"/>
-    <hyperlink ref="H59" r:id="rId53" xr:uid="{2AAD2FC9-7875-4C7E-BE18-5929DCD300E2}"/>
-    <hyperlink ref="H60" r:id="rId54" xr:uid="{3B13B48B-CFD8-43FD-A256-BFBCA6E9F166}"/>
-    <hyperlink ref="H61" r:id="rId55" xr:uid="{2812F3C5-BA5B-4280-A6EE-F071C743A0F9}"/>
-    <hyperlink ref="H62" r:id="rId56" xr:uid="{A51391BB-726E-4E53-A854-F835E4326CB7}"/>
-    <hyperlink ref="H63" r:id="rId57" xr:uid="{3816078E-236A-40ED-8098-8D6C2593073C}"/>
-    <hyperlink ref="H64" r:id="rId58" xr:uid="{16019511-2A5B-45DB-9951-7580C7CED611}"/>
-    <hyperlink ref="H65" r:id="rId59" xr:uid="{0F281052-88CC-4EFC-9654-D738A5265195}"/>
-    <hyperlink ref="H66" r:id="rId60" xr:uid="{988320DB-75EE-40A5-80AB-5DC5D88C77B3}"/>
-    <hyperlink ref="H67" r:id="rId61" xr:uid="{BD69E281-B932-4E39-BC3D-0A5839B363E1}"/>
-    <hyperlink ref="H68" r:id="rId62" xr:uid="{E063F8A8-C725-4BE8-8357-391DBDD95480}"/>
-    <hyperlink ref="H69" r:id="rId63" xr:uid="{46926277-A148-4D82-AF7C-43360CBCA36A}"/>
-    <hyperlink ref="G11" r:id="rId64" xr:uid="{08891F1E-BFCE-4901-BB79-93AA85608BD6}"/>
-    <hyperlink ref="G12" r:id="rId65" xr:uid="{5B945965-8CF2-4536-B6C6-B03AA77AC55C}"/>
-    <hyperlink ref="G13" r:id="rId66" xr:uid="{474F2900-37DB-45FC-AC64-A44473756317}"/>
-    <hyperlink ref="G14" r:id="rId67" xr:uid="{8083D30B-557A-4AC8-8D3C-27A3DD20F6F0}"/>
-    <hyperlink ref="G15" r:id="rId68" xr:uid="{9BC24074-15A2-42CF-82F3-9EE884921304}"/>
-    <hyperlink ref="G16" r:id="rId69" xr:uid="{CC4BD510-687D-4365-A02B-40308B7BB094}"/>
-    <hyperlink ref="G17" r:id="rId70" xr:uid="{307F9D09-DD1B-449E-8BD1-CEA8554CE58F}"/>
-    <hyperlink ref="G18" r:id="rId71" xr:uid="{256E56A0-313B-40C0-B777-463B070E8BC5}"/>
-    <hyperlink ref="G19" r:id="rId72" xr:uid="{53093AA6-4084-4A8D-9497-0ED7AA03C383}"/>
-    <hyperlink ref="G20" r:id="rId73" xr:uid="{0A61BB15-6DA2-4651-832C-63B5FBFBF363}"/>
-    <hyperlink ref="G21" r:id="rId74" xr:uid="{81605D05-A6AE-48A8-B253-5F4DDBDA4ADF}"/>
-    <hyperlink ref="G22" r:id="rId75" xr:uid="{CC010305-21EE-4FDA-9CD9-E1E88E21073E}"/>
-    <hyperlink ref="G23" r:id="rId76" xr:uid="{015C4D36-070E-4AE5-8A75-18BB99358F8A}"/>
-    <hyperlink ref="G24" r:id="rId77" xr:uid="{9388E673-BA81-47E0-BFEB-FD5D9EFB6189}"/>
-    <hyperlink ref="G25" r:id="rId78" xr:uid="{C35AD358-FAE5-4651-BA71-7FCB62B777AD}"/>
-    <hyperlink ref="G26" r:id="rId79" xr:uid="{49164CC9-A989-48A1-907E-506CF71CAD23}"/>
-    <hyperlink ref="G27" r:id="rId80" xr:uid="{FD0CC0A5-6781-4196-BC44-A37E10AEC42E}"/>
-    <hyperlink ref="G28" r:id="rId81" xr:uid="{EEC82DBC-4EC1-4487-B9D7-395DEF439593}"/>
-    <hyperlink ref="G29" r:id="rId82" xr:uid="{D76B3FB4-0C70-4CE6-918B-0908E0F374B8}"/>
-    <hyperlink ref="G30" r:id="rId83" xr:uid="{1DEFF231-CA99-4D17-8AE5-615AC7A823A4}"/>
-    <hyperlink ref="G31" r:id="rId84" xr:uid="{966D5DAB-BC05-48B1-AED4-A984DDFA9687}"/>
-    <hyperlink ref="G32" r:id="rId85" xr:uid="{89CC95B8-463D-4ED6-BCD0-BD61431EEC6B}"/>
-    <hyperlink ref="G33" r:id="rId86" xr:uid="{59E52C85-2003-40A5-8C17-8E2F50167809}"/>
-    <hyperlink ref="G34" r:id="rId87" xr:uid="{BA71EEF9-AF74-4964-81CA-5687E31C1DD4}"/>
-    <hyperlink ref="G35" r:id="rId88" xr:uid="{D4B8B830-7DBB-47C0-A575-21C20C37106F}"/>
-    <hyperlink ref="G36" r:id="rId89" xr:uid="{A3B66E16-DF2D-4C8E-8493-576C3B334E63}"/>
-    <hyperlink ref="G37" r:id="rId90" xr:uid="{A8760C98-A87A-41BC-846D-7C27B64DC83F}"/>
-    <hyperlink ref="G38" r:id="rId91" xr:uid="{A325DB0A-16B9-4C9B-AD23-028436D268E4}"/>
-    <hyperlink ref="G39" r:id="rId92" xr:uid="{21E4E18D-D7B0-4619-9131-F214640DD643}"/>
-    <hyperlink ref="G40" r:id="rId93" xr:uid="{BB72CDF5-7DBF-4D40-BD56-FA7B73CD3590}"/>
-    <hyperlink ref="G41" r:id="rId94" xr:uid="{0755F9B0-B3FA-4412-9627-511B01D587C4}"/>
-    <hyperlink ref="G42" r:id="rId95" xr:uid="{0E77696F-C2A8-46A4-A1C9-5B053BCCD56A}"/>
-    <hyperlink ref="G43" r:id="rId96" xr:uid="{62AD8424-5EED-4E05-BD4A-67FFF079F5DE}"/>
-    <hyperlink ref="G44" r:id="rId97" xr:uid="{BD5F52DA-750A-4708-9209-F0832953610C}"/>
-    <hyperlink ref="G45" r:id="rId98" xr:uid="{5DB21C96-F541-4875-82E0-FD95E99F7A16}"/>
-    <hyperlink ref="G46" r:id="rId99" xr:uid="{3296534A-C4DB-4629-8892-2512BE67C1E1}"/>
-    <hyperlink ref="G47" r:id="rId100" xr:uid="{FC4C2567-5D0A-4A46-87FD-0F052C0C538D}"/>
-    <hyperlink ref="G48" r:id="rId101" xr:uid="{CCBD4575-042B-483B-B95F-DB0C6BFBBF8D}"/>
-    <hyperlink ref="G49" r:id="rId102" xr:uid="{433D9299-B965-440B-AB9D-D1BC0FF90227}"/>
-    <hyperlink ref="G50" r:id="rId103" xr:uid="{9C92CA39-C795-4745-BCA7-75F9635352EF}"/>
-    <hyperlink ref="G51" r:id="rId104" xr:uid="{80955053-99B6-4770-9451-1AB0C4AB0658}"/>
-    <hyperlink ref="G52" r:id="rId105" xr:uid="{D08F8A10-1FEA-4FF8-91AA-4D5C6E2CF965}"/>
-    <hyperlink ref="G53" r:id="rId106" xr:uid="{E1552DE5-3F36-4447-A098-1C38DEF076C3}"/>
-    <hyperlink ref="G54" r:id="rId107" xr:uid="{27C89CBD-A689-49D7-A356-45AB8D080E30}"/>
-    <hyperlink ref="G55" r:id="rId108" xr:uid="{71744331-B135-4284-A969-858AB98596A0}"/>
-    <hyperlink ref="G56" r:id="rId109" xr:uid="{E8227959-A688-47B5-8A00-EAAE316BCF25}"/>
-    <hyperlink ref="G57" r:id="rId110" xr:uid="{81A75D53-81AF-47EF-955C-7F6AE6E8D441}"/>
-    <hyperlink ref="G58" r:id="rId111" xr:uid="{381AF0E9-4678-4C36-98E5-18D44A2CC57D}"/>
-    <hyperlink ref="G59" r:id="rId112" xr:uid="{851C0207-0075-4165-8E96-8EDBA705D1BE}"/>
-    <hyperlink ref="G60" r:id="rId113" xr:uid="{0EB71C1A-846F-471B-A44E-D6A98021B2BD}"/>
-    <hyperlink ref="G61" r:id="rId114" xr:uid="{015E38E2-E0E0-4C07-9DC8-737D165A1996}"/>
-    <hyperlink ref="G62" r:id="rId115" xr:uid="{403E4063-551A-486E-A1F9-3F42AF284878}"/>
-    <hyperlink ref="G63" r:id="rId116" xr:uid="{4B58B3D6-A744-4480-9F2D-E188A123B412}"/>
-    <hyperlink ref="G64" r:id="rId117" xr:uid="{8042DD29-EA9B-4FD4-82D4-4821278FDA07}"/>
-    <hyperlink ref="G65" r:id="rId118" xr:uid="{C726FBED-BFBE-4CE0-96C2-8969080BF41C}"/>
-    <hyperlink ref="G66" r:id="rId119" xr:uid="{A7FDEECE-9C08-46A0-9503-19049D241A3B}"/>
-    <hyperlink ref="G67" r:id="rId120" xr:uid="{8A8FED6A-5191-4D66-9581-4022B7D0D290}"/>
-    <hyperlink ref="G68" r:id="rId121" xr:uid="{A08C4575-38E9-451E-80D2-24708329B4C0}"/>
-    <hyperlink ref="G69" r:id="rId122" xr:uid="{72CA6DCC-6E4F-454E-BE85-9513BC2C22F5}"/>
+    <hyperlink ref="H2" r:id="rId2" display="nayrpkt@gmail.com" xr:uid="{FCA25B0F-6286-4320-9B1F-FD5A64DBBEB1}"/>
+    <hyperlink ref="G3:G10" r:id="rId3" display="robert.ads.anjos@gmail.com" xr:uid="{00541651-9D2B-43BD-B943-758F742CF890}"/>
+    <hyperlink ref="G11" r:id="rId4" xr:uid="{08891F1E-BFCE-4901-BB79-93AA85608BD6}"/>
+    <hyperlink ref="G12" r:id="rId5" xr:uid="{5B945965-8CF2-4536-B6C6-B03AA77AC55C}"/>
+    <hyperlink ref="G13" r:id="rId6" xr:uid="{474F2900-37DB-45FC-AC64-A44473756317}"/>
+    <hyperlink ref="G14" r:id="rId7" xr:uid="{8083D30B-557A-4AC8-8D3C-27A3DD20F6F0}"/>
+    <hyperlink ref="G15" r:id="rId8" xr:uid="{9BC24074-15A2-42CF-82F3-9EE884921304}"/>
+    <hyperlink ref="G16" r:id="rId9" xr:uid="{CC4BD510-687D-4365-A02B-40308B7BB094}"/>
+    <hyperlink ref="G17" r:id="rId10" xr:uid="{307F9D09-DD1B-449E-8BD1-CEA8554CE58F}"/>
+    <hyperlink ref="G18" r:id="rId11" xr:uid="{256E56A0-313B-40C0-B777-463B070E8BC5}"/>
+    <hyperlink ref="G19" r:id="rId12" xr:uid="{53093AA6-4084-4A8D-9497-0ED7AA03C383}"/>
+    <hyperlink ref="G20" r:id="rId13" xr:uid="{0A61BB15-6DA2-4651-832C-63B5FBFBF363}"/>
+    <hyperlink ref="G21" r:id="rId14" xr:uid="{81605D05-A6AE-48A8-B253-5F4DDBDA4ADF}"/>
+    <hyperlink ref="G22" r:id="rId15" xr:uid="{CC010305-21EE-4FDA-9CD9-E1E88E21073E}"/>
+    <hyperlink ref="G23" r:id="rId16" xr:uid="{015C4D36-070E-4AE5-8A75-18BB99358F8A}"/>
+    <hyperlink ref="G24" r:id="rId17" xr:uid="{9388E673-BA81-47E0-BFEB-FD5D9EFB6189}"/>
+    <hyperlink ref="G25" r:id="rId18" xr:uid="{C35AD358-FAE5-4651-BA71-7FCB62B777AD}"/>
+    <hyperlink ref="G26" r:id="rId19" xr:uid="{49164CC9-A989-48A1-907E-506CF71CAD23}"/>
+    <hyperlink ref="G27" r:id="rId20" xr:uid="{FD0CC0A5-6781-4196-BC44-A37E10AEC42E}"/>
+    <hyperlink ref="G28" r:id="rId21" xr:uid="{EEC82DBC-4EC1-4487-B9D7-395DEF439593}"/>
+    <hyperlink ref="G29" r:id="rId22" xr:uid="{D76B3FB4-0C70-4CE6-918B-0908E0F374B8}"/>
+    <hyperlink ref="G30" r:id="rId23" xr:uid="{1DEFF231-CA99-4D17-8AE5-615AC7A823A4}"/>
+    <hyperlink ref="G31" r:id="rId24" xr:uid="{966D5DAB-BC05-48B1-AED4-A984DDFA9687}"/>
+    <hyperlink ref="G32" r:id="rId25" xr:uid="{89CC95B8-463D-4ED6-BCD0-BD61431EEC6B}"/>
+    <hyperlink ref="G33" r:id="rId26" xr:uid="{59E52C85-2003-40A5-8C17-8E2F50167809}"/>
+    <hyperlink ref="G34" r:id="rId27" xr:uid="{BA71EEF9-AF74-4964-81CA-5687E31C1DD4}"/>
+    <hyperlink ref="G35" r:id="rId28" xr:uid="{D4B8B830-7DBB-47C0-A575-21C20C37106F}"/>
+    <hyperlink ref="G36" r:id="rId29" xr:uid="{A3B66E16-DF2D-4C8E-8493-576C3B334E63}"/>
+    <hyperlink ref="G37" r:id="rId30" xr:uid="{A8760C98-A87A-41BC-846D-7C27B64DC83F}"/>
+    <hyperlink ref="G38" r:id="rId31" xr:uid="{A325DB0A-16B9-4C9B-AD23-028436D268E4}"/>
+    <hyperlink ref="G39" r:id="rId32" xr:uid="{21E4E18D-D7B0-4619-9131-F214640DD643}"/>
+    <hyperlink ref="G40" r:id="rId33" xr:uid="{BB72CDF5-7DBF-4D40-BD56-FA7B73CD3590}"/>
+    <hyperlink ref="G41" r:id="rId34" xr:uid="{0755F9B0-B3FA-4412-9627-511B01D587C4}"/>
+    <hyperlink ref="G42" r:id="rId35" xr:uid="{0E77696F-C2A8-46A4-A1C9-5B053BCCD56A}"/>
+    <hyperlink ref="G43" r:id="rId36" xr:uid="{62AD8424-5EED-4E05-BD4A-67FFF079F5DE}"/>
+    <hyperlink ref="G44" r:id="rId37" xr:uid="{BD5F52DA-750A-4708-9209-F0832953610C}"/>
+    <hyperlink ref="G45" r:id="rId38" xr:uid="{5DB21C96-F541-4875-82E0-FD95E99F7A16}"/>
+    <hyperlink ref="G46" r:id="rId39" xr:uid="{3296534A-C4DB-4629-8892-2512BE67C1E1}"/>
+    <hyperlink ref="G47" r:id="rId40" xr:uid="{FC4C2567-5D0A-4A46-87FD-0F052C0C538D}"/>
+    <hyperlink ref="G48" r:id="rId41" xr:uid="{CCBD4575-042B-483B-B95F-DB0C6BFBBF8D}"/>
+    <hyperlink ref="G49" r:id="rId42" xr:uid="{433D9299-B965-440B-AB9D-D1BC0FF90227}"/>
+    <hyperlink ref="G50" r:id="rId43" xr:uid="{9C92CA39-C795-4745-BCA7-75F9635352EF}"/>
+    <hyperlink ref="G51" r:id="rId44" xr:uid="{80955053-99B6-4770-9451-1AB0C4AB0658}"/>
+    <hyperlink ref="G52" r:id="rId45" xr:uid="{D08F8A10-1FEA-4FF8-91AA-4D5C6E2CF965}"/>
+    <hyperlink ref="G53" r:id="rId46" xr:uid="{E1552DE5-3F36-4447-A098-1C38DEF076C3}"/>
+    <hyperlink ref="G54" r:id="rId47" xr:uid="{27C89CBD-A689-49D7-A356-45AB8D080E30}"/>
+    <hyperlink ref="G55" r:id="rId48" xr:uid="{71744331-B135-4284-A969-858AB98596A0}"/>
+    <hyperlink ref="G56" r:id="rId49" xr:uid="{E8227959-A688-47B5-8A00-EAAE316BCF25}"/>
+    <hyperlink ref="G57" r:id="rId50" xr:uid="{81A75D53-81AF-47EF-955C-7F6AE6E8D441}"/>
+    <hyperlink ref="G58" r:id="rId51" xr:uid="{381AF0E9-4678-4C36-98E5-18D44A2CC57D}"/>
+    <hyperlink ref="G59" r:id="rId52" xr:uid="{851C0207-0075-4165-8E96-8EDBA705D1BE}"/>
+    <hyperlink ref="G60" r:id="rId53" xr:uid="{0EB71C1A-846F-471B-A44E-D6A98021B2BD}"/>
+    <hyperlink ref="G61" r:id="rId54" xr:uid="{015E38E2-E0E0-4C07-9DC8-737D165A1996}"/>
+    <hyperlink ref="G62" r:id="rId55" xr:uid="{403E4063-551A-486E-A1F9-3F42AF284878}"/>
+    <hyperlink ref="G63" r:id="rId56" xr:uid="{4B58B3D6-A744-4480-9F2D-E188A123B412}"/>
+    <hyperlink ref="G64" r:id="rId57" xr:uid="{8042DD29-EA9B-4FD4-82D4-4821278FDA07}"/>
+    <hyperlink ref="G65" r:id="rId58" xr:uid="{C726FBED-BFBE-4CE0-96C2-8969080BF41C}"/>
+    <hyperlink ref="G66" r:id="rId59" xr:uid="{A7FDEECE-9C08-46A0-9503-19049D241A3B}"/>
+    <hyperlink ref="G67" r:id="rId60" xr:uid="{8A8FED6A-5191-4D66-9581-4022B7D0D290}"/>
+    <hyperlink ref="G68" r:id="rId61" xr:uid="{A08C4575-38E9-451E-80D2-24708329B4C0}"/>
+    <hyperlink ref="G69" r:id="rId62" xr:uid="{72CA6DCC-6E4F-454E-BE85-9513BC2C22F5}"/>
+    <hyperlink ref="H3:H20" r:id="rId63" display="nayrpkt@gmail.com" xr:uid="{A9CFD133-3D0E-43E2-851B-11CE749C6EB0}"/>
+    <hyperlink ref="H20" r:id="rId64" xr:uid="{81BF9F93-7261-4477-8CAC-7952CFC7B75D}"/>
+    <hyperlink ref="H21:H69" r:id="rId65" display="nayrpkt@gmail.com" xr:uid="{1C7B856C-4B88-489F-9FA7-AAF47B464C4A}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId123"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Criando método para tratar as cópias e incluindo + try
</commit_message>
<xml_diff>
--- a/Mensageria/betti/email.xlsx
+++ b/Mensageria/betti/email.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robert.alves\source\aulas\AulasEuCodo\Mensageria\betti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECEB8B-8EB5-47B6-A844-C7DB66593508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB20613-ECD9-4C17-A683-0F125ECD2002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B2C2596-FEDC-4806-AA04-C3A6BED56956}"/>
   </bookViews>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59491F56-CD08-47F1-9229-800FA97E9013}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>